<commit_message>
Rotated Pls & Rtn switches, they are loose in the plate in original orientation
</commit_message>
<xml_diff>
--- a/Numpad-BoM.xlsx
+++ b/Numpad-BoM.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Keyboard\pcbs\numpad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{173426CF-0EE4-4E45-A00D-7E7D716156C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE551812-7D2E-4F49-AFF3-A43B86C73C00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="38280" yWindow="780" windowWidth="15600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numpad" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
-  <si>
-    <t xml:space="preserve">C1 </t>
-  </si>
-  <si>
-    <t>100nF</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="70">
   <si>
     <t>Capacitor_SMD:C_0603_1608Metric_Pad1.05x0.95mm_HandSolder</t>
   </si>
@@ -241,7 +235,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1077,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,24 +1083,25 @@
     <col min="1" max="1" width="44" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="104.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,16 +1109,19 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>63</v>
+      </c>
+      <c r="G2">
+        <v>805</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1137,10 +1135,10 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3">
         <v>805</v>
@@ -1148,124 +1146,118 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4">
-        <v>805</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
-        <v>17</v>
+      <c r="C8">
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <v>330</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>330</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1276,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>22</v>
@@ -1290,122 +1282,122 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>32</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20">
-        <v>9</v>
-      </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1419,7 +1411,7 @@
         <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1433,7 +1425,7 @@
         <v>36</v>
       </c>
       <c r="D22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,21 +1439,21 @@
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,7 +1467,7 @@
         <v>43</v>
       </c>
       <c r="D25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1489,7 +1481,7 @@
         <v>45</v>
       </c>
       <c r="D26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1503,7 +1495,7 @@
         <v>47</v>
       </c>
       <c r="D27" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1514,72 +1506,58 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>50</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
       <c r="D29" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
         <v>57</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>59</v>
-      </c>
-      <c r="F32" t="s">
-        <v>71</v>
+      <c r="F31" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>